<commit_message>
Add middle squares. Add custom parameters
</commit_message>
<xml_diff>
--- a/Sample Data.xlsx
+++ b/Sample Data.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="93">
   <si>
     <t>pig</t>
   </si>
@@ -185,118 +185,130 @@
     <t>square 5</t>
   </si>
   <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>border</t>
+  </si>
+  <si>
+    <t>card_number</t>
+  </si>
+  <si>
+    <t>001</t>
+  </si>
+  <si>
+    <t>002</t>
+  </si>
+  <si>
+    <t>003</t>
+  </si>
+  <si>
+    <t>004</t>
+  </si>
+  <si>
+    <t>005</t>
+  </si>
+  <si>
+    <t>006</t>
+  </si>
+  <si>
+    <t>007</t>
+  </si>
+  <si>
+    <t>008</t>
+  </si>
+  <si>
+    <t>009</t>
+  </si>
+  <si>
+    <t>010</t>
+  </si>
+  <si>
+    <t>011</t>
+  </si>
+  <si>
+    <t>012</t>
+  </si>
+  <si>
+    <t>013</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>pig.jpg</t>
+  </si>
+  <si>
+    <t>bear.jpg</t>
+  </si>
+  <si>
+    <t>bird.jpg</t>
+  </si>
+  <si>
+    <t>butterfly.jpg</t>
+  </si>
+  <si>
+    <t>cat.jpg</t>
+  </si>
+  <si>
+    <t>chicken.jpg</t>
+  </si>
+  <si>
+    <t>cow.jpg</t>
+  </si>
+  <si>
+    <t>dog.jpg</t>
+  </si>
+  <si>
+    <t>donkey.jpg</t>
+  </si>
+  <si>
+    <t>duck.jpg</t>
+  </si>
+  <si>
+    <t>eagle.jpg</t>
+  </si>
+  <si>
+    <t>mouse.jpg</t>
+  </si>
+  <si>
+    <t>rabbit.jpg</t>
+  </si>
+  <si>
+    <t>terra_orange.jpg</t>
+  </si>
+  <si>
+    <t>terra_green.jpg</t>
+  </si>
+  <si>
+    <t>terra_blue.jpg</t>
+  </si>
+  <si>
+    <t>terra_purple.jpg</t>
+  </si>
+  <si>
+    <t>3Y</t>
+  </si>
+  <si>
+    <t>4Z</t>
+  </si>
+  <si>
+    <t>rock.png</t>
+  </si>
+  <si>
     <t>scissors.png</t>
   </si>
   <si>
     <t>paper.png</t>
   </si>
   <si>
-    <t>rock.png</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>border</t>
-  </si>
-  <si>
-    <t>card_number</t>
-  </si>
-  <si>
-    <t>001</t>
-  </si>
-  <si>
-    <t>002</t>
-  </si>
-  <si>
-    <t>003</t>
-  </si>
-  <si>
-    <t>004</t>
-  </si>
-  <si>
-    <t>005</t>
-  </si>
-  <si>
-    <t>006</t>
-  </si>
-  <si>
-    <t>007</t>
-  </si>
-  <si>
-    <t>008</t>
-  </si>
-  <si>
-    <t>009</t>
-  </si>
-  <si>
-    <t>010</t>
-  </si>
-  <si>
-    <t>011</t>
-  </si>
-  <si>
-    <t>012</t>
-  </si>
-  <si>
-    <t>013</t>
-  </si>
-  <si>
-    <t>V</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>pig.jpg</t>
-  </si>
-  <si>
-    <t>bear.jpg</t>
-  </si>
-  <si>
-    <t>bird.jpg</t>
-  </si>
-  <si>
-    <t>butterfly.jpg</t>
-  </si>
-  <si>
-    <t>cat.jpg</t>
-  </si>
-  <si>
-    <t>chicken.jpg</t>
-  </si>
-  <si>
-    <t>cow.jpg</t>
-  </si>
-  <si>
-    <t>dog.jpg</t>
-  </si>
-  <si>
-    <t>donkey.jpg</t>
-  </si>
-  <si>
-    <t>duck.jpg</t>
-  </si>
-  <si>
-    <t>eagle.jpg</t>
-  </si>
-  <si>
-    <t>mouse.jpg</t>
-  </si>
-  <si>
-    <t>rabbit.jpg</t>
-  </si>
-  <si>
-    <t>terra_orange.png</t>
-  </si>
-  <si>
-    <t>terra_green.png</t>
-  </si>
-  <si>
-    <t>terra_blue.png</t>
-  </si>
-  <si>
-    <t>terra_purple.png</t>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>XYZ</t>
   </si>
 </sst>
 </file>
@@ -686,15 +698,15 @@
     <col min="4" max="4" width="12" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>15</v>
@@ -727,12 +739,12 @@
         <v>50</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>19</v>
@@ -747,21 +759,24 @@
         <v>2</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>53</v>
+        <v>88</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>19</v>
@@ -776,21 +791,27 @@
         <v>22</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="I3" s="1" t="s">
-        <v>54</v>
+      <c r="J3" s="1">
+        <v>36</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>19</v>
@@ -805,21 +826,21 @@
         <v>24</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>52</v>
+        <v>71</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>90</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>20</v>
@@ -834,21 +855,21 @@
         <v>26</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>19</v>
@@ -863,21 +884,21 @@
         <v>28</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G6" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="I6" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="L6" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>19</v>
@@ -892,21 +913,24 @@
         <v>30</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>52</v>
+        <v>90</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>19</v>
@@ -921,24 +945,24 @@
         <v>32</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>53</v>
+        <v>88</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>52</v>
+        <v>90</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>19</v>
@@ -953,24 +977,24 @@
         <v>34</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>51</v>
+        <v>89</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>53</v>
+        <v>88</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>19</v>
@@ -985,24 +1009,24 @@
         <v>36</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>52</v>
+        <v>90</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="K10" s="1">
-        <v>2</v>
+        <v>68</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>19</v>
@@ -1017,21 +1041,27 @@
         <v>38</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>53</v>
+        <v>88</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>90</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
+      </c>
+      <c r="J11" s="1">
+        <v>20</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>19</v>
@@ -1046,21 +1076,21 @@
         <v>40</v>
       </c>
       <c r="F12" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="L12" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>19</v>
@@ -1075,21 +1105,30 @@
         <v>42</v>
       </c>
       <c r="F13" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J13" s="1">
+        <v>40</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="L13" s="1" t="s">
         <v>83</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>19</v>
@@ -1104,16 +1143,22 @@
         <v>44</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>53</v>
+        <v>88</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>92</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>87</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Solve white dots on border issue
</commit_message>
<xml_diff>
--- a/Sample Data.xlsx
+++ b/Sample Data.xlsx
@@ -188,96 +188,117 @@
     <t>N</t>
   </si>
   <si>
+    <t>card_number</t>
+  </si>
+  <si>
+    <t>001</t>
+  </si>
+  <si>
+    <t>002</t>
+  </si>
+  <si>
+    <t>003</t>
+  </si>
+  <si>
+    <t>004</t>
+  </si>
+  <si>
+    <t>005</t>
+  </si>
+  <si>
+    <t>006</t>
+  </si>
+  <si>
+    <t>007</t>
+  </si>
+  <si>
+    <t>008</t>
+  </si>
+  <si>
+    <t>009</t>
+  </si>
+  <si>
+    <t>010</t>
+  </si>
+  <si>
+    <t>011</t>
+  </si>
+  <si>
+    <t>012</t>
+  </si>
+  <si>
+    <t>013</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>pig.jpg</t>
+  </si>
+  <si>
+    <t>bear.jpg</t>
+  </si>
+  <si>
+    <t>bird.jpg</t>
+  </si>
+  <si>
+    <t>butterfly.jpg</t>
+  </si>
+  <si>
+    <t>cat.jpg</t>
+  </si>
+  <si>
+    <t>chicken.jpg</t>
+  </si>
+  <si>
+    <t>cow.jpg</t>
+  </si>
+  <si>
+    <t>dog.jpg</t>
+  </si>
+  <si>
+    <t>donkey.jpg</t>
+  </si>
+  <si>
+    <t>duck.jpg</t>
+  </si>
+  <si>
+    <t>eagle.jpg</t>
+  </si>
+  <si>
+    <t>mouse.jpg</t>
+  </si>
+  <si>
+    <t>rabbit.jpg</t>
+  </si>
+  <si>
+    <t>3Y</t>
+  </si>
+  <si>
+    <t>4Z</t>
+  </si>
+  <si>
+    <t>rock.png</t>
+  </si>
+  <si>
+    <t>scissors.png</t>
+  </si>
+  <si>
+    <t>paper.png</t>
+  </si>
+  <si>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>XYZ</t>
+  </si>
+  <si>
     <t>border</t>
   </si>
   <si>
-    <t>card_number</t>
-  </si>
-  <si>
-    <t>001</t>
-  </si>
-  <si>
-    <t>002</t>
-  </si>
-  <si>
-    <t>003</t>
-  </si>
-  <si>
-    <t>004</t>
-  </si>
-  <si>
-    <t>005</t>
-  </si>
-  <si>
-    <t>006</t>
-  </si>
-  <si>
-    <t>007</t>
-  </si>
-  <si>
-    <t>008</t>
-  </si>
-  <si>
-    <t>009</t>
-  </si>
-  <si>
-    <t>010</t>
-  </si>
-  <si>
-    <t>011</t>
-  </si>
-  <si>
-    <t>012</t>
-  </si>
-  <si>
-    <t>013</t>
-  </si>
-  <si>
-    <t>V</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>pig.jpg</t>
-  </si>
-  <si>
-    <t>bear.jpg</t>
-  </si>
-  <si>
-    <t>bird.jpg</t>
-  </si>
-  <si>
-    <t>butterfly.jpg</t>
-  </si>
-  <si>
-    <t>cat.jpg</t>
-  </si>
-  <si>
-    <t>chicken.jpg</t>
-  </si>
-  <si>
-    <t>cow.jpg</t>
-  </si>
-  <si>
-    <t>dog.jpg</t>
-  </si>
-  <si>
-    <t>donkey.jpg</t>
-  </si>
-  <si>
-    <t>duck.jpg</t>
-  </si>
-  <si>
-    <t>eagle.jpg</t>
-  </si>
-  <si>
-    <t>mouse.jpg</t>
-  </si>
-  <si>
-    <t>rabbit.jpg</t>
-  </si>
-  <si>
     <t>terra_orange.jpg</t>
   </si>
   <si>
@@ -288,27 +309,6 @@
   </si>
   <si>
     <t>terra_purple.jpg</t>
-  </si>
-  <si>
-    <t>3Y</t>
-  </si>
-  <si>
-    <t>4Z</t>
-  </si>
-  <si>
-    <t>rock.png</t>
-  </si>
-  <si>
-    <t>scissors.png</t>
-  </si>
-  <si>
-    <t>paper.png</t>
-  </si>
-  <si>
-    <t>ABC</t>
-  </si>
-  <si>
-    <t>XYZ</t>
   </si>
 </sst>
 </file>
@@ -706,7 +706,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>15</v>
@@ -739,12 +739,12 @@
         <v>50</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>52</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>19</v>
@@ -759,24 +759,24 @@
         <v>2</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>51</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>19</v>
@@ -791,13 +791,13 @@
         <v>22</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>51</v>
@@ -806,12 +806,12 @@
         <v>36</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>19</v>
@@ -826,21 +826,21 @@
         <v>24</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>51</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>20</v>
@@ -855,21 +855,21 @@
         <v>26</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>51</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>19</v>
@@ -884,21 +884,21 @@
         <v>28</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>51</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>19</v>
@@ -913,24 +913,24 @@
         <v>30</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>51</v>
       </c>
       <c r="K7" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="L7" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>19</v>
@@ -945,24 +945,24 @@
         <v>32</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>19</v>
@@ -977,24 +977,24 @@
         <v>34</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>19</v>
@@ -1009,24 +1009,24 @@
         <v>36</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>19</v>
@@ -1041,13 +1041,13 @@
         <v>38</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>51</v>
@@ -1056,12 +1056,12 @@
         <v>20</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>19</v>
@@ -1076,21 +1076,21 @@
         <v>40</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>51</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>19</v>
@@ -1105,13 +1105,13 @@
         <v>42</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>51</v>
@@ -1120,15 +1120,15 @@
         <v>40</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>19</v>
@@ -1143,22 +1143,22 @@
         <v>44</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>51</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>83</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>